<commit_message>
ajout doc boite à fusible avant
</commit_message>
<xml_diff>
--- a/EL_Electrical/Gearshift/Suivi_Gearshift Controller.xlsx
+++ b/EL_Electrical/Gearshift/Suivi_Gearshift Controller.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6D0502-49CF-47A5-B86B-85553121CC6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1077C01-EE28-4F8B-A7D6-8850C7700839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="9390" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Généralités" sheetId="8" r:id="rId1"/>
@@ -138,10 +138,10 @@
     <t>Bruno Moreira Nabinger</t>
   </si>
   <si>
-    <t>Envoyer les commandes pour passer les vitesse selon les commandes des palettes</t>
+    <t>à définir</t>
   </si>
   <si>
-    <t>à définir</t>
+    <t>Envoyer les commandes pour passer les vitesses selon les commandes des palettes</t>
   </si>
 </sst>
 </file>
@@ -584,6 +584,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -596,15 +603,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -612,30 +621,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -652,30 +676,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1620,8 +1620,8 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:F21"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,65 +1633,65 @@
       <c r="A1" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="52" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="51" t="s">
-        <v>35</v>
+      <c r="B9" s="53"/>
+      <c r="C9" s="54" t="s">
+        <v>36</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -1703,174 +1703,158 @@
       <c r="H13" s="11"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="54" t="s">
-        <v>36</v>
+      <c r="B20" s="50"/>
+      <c r="C20" s="48" t="s">
+        <v>35</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="48"/>
+      <c r="B33" s="51"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="52" t="s">
+      <c r="B34" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="F34" s="54" t="s">
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="F34" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="F35" s="54" t="s">
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="F35" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="F36" s="54" t="s">
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="F36" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="F37" s="54" t="s">
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="F37" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B34:D34"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
@@ -1887,6 +1871,22 @@
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C27:H28"/>
     <mergeCell ref="C16:H16"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1927,8 +1927,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
@@ -1936,8 +1936,8 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="19"/>
@@ -1950,9 +1950,9 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
       <c r="F4" s="17"/>
@@ -1963,8 +1963,8 @@
       <c r="N4" s="25"/>
     </row>
     <row r="5" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="18"/>
@@ -1976,12 +1976,12 @@
       <c r="N5" s="25"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
       <c r="H6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="25"/>
@@ -1989,32 +1989,32 @@
       <c r="N6" s="25"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="H7" s="6"/>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
       <c r="H8" s="6"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:16" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2028,9 +2028,9 @@
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
       <c r="E12" s="6"/>
       <c r="G12" s="3"/>
       <c r="H12" s="6"/>
@@ -2041,55 +2041,55 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
     </row>
     <row r="18" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2097,58 +2097,58 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="57"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="57"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
+      <c r="A24" s="60"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="57"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2156,28 +2156,28 @@
       <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="57"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
+      <c r="A31" s="60"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="57"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2195,44 +2195,44 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="57"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="57"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="57"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
+      <c r="A38" s="60"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="57"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
+      <c r="A39" s="60"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="60"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="57"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="57"/>
+      <c r="A40" s="60"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
@@ -2260,11 +2260,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:F9"/>
-    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A30:F32"/>
     <mergeCell ref="A36:F40"/>
@@ -2272,6 +2267,11 @@
     <mergeCell ref="A14:F18"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:F27"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:F9"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.38825757575757575" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2307,19 +2307,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
+      <c r="A1" s="73"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
       <c r="D2" s="10"/>
       <c r="E2" s="9"/>
       <c r="N2" s="10"/>
@@ -2330,10 +2330,10 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="45" t="s">
         <v>20</v>
       </c>
@@ -2351,8 +2351,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="43"/>
       <c r="D5" s="44"/>
       <c r="E5" s="44"/>
@@ -2360,8 +2360,8 @@
       <c r="G5" s="44"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70"/>
-      <c r="B6" s="71"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="30"/>
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
@@ -2369,8 +2369,8 @@
       <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
-      <c r="B7" s="63"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="23"/>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
@@ -2378,8 +2378,8 @@
       <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="63"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="23"/>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -2387,8 +2387,8 @@
       <c r="G8" s="29"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="63"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="26"/>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -2396,8 +2396,8 @@
       <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="23"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
@@ -2405,8 +2405,8 @@
       <c r="G10" s="29"/>
     </row>
     <row r="11" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="23"/>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
@@ -2414,8 +2414,8 @@
       <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
-      <c r="B12" s="63"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="26"/>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
@@ -2423,8 +2423,8 @@
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="26"/>
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
@@ -2432,8 +2432,8 @@
       <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
-      <c r="B14" s="73"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
@@ -2441,8 +2441,8 @@
       <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
-      <c r="B15" s="63"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="26"/>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
@@ -2450,8 +2450,8 @@
       <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
-      <c r="B16" s="63"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="23"/>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
@@ -2459,8 +2459,8 @@
       <c r="G16" s="29"/>
     </row>
     <row r="17" spans="1:8" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="23"/>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
@@ -2468,8 +2468,8 @@
       <c r="G17" s="29"/>
     </row>
     <row r="18" spans="1:8" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
-      <c r="B18" s="63"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="23"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
@@ -2478,8 +2478,8 @@
       <c r="H18" s="27"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
-      <c r="B19" s="63"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="23"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
@@ -2488,8 +2488,8 @@
       <c r="H19" s="27"/>
     </row>
     <row r="20" spans="1:8" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="63"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="23"/>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
@@ -2498,8 +2498,8 @@
       <c r="H20" s="27"/>
     </row>
     <row r="21" spans="1:8" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
-      <c r="B21" s="63"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="23"/>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
@@ -2508,8 +2508,8 @@
       <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
-      <c r="B22" s="63"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="23"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
@@ -2534,11 +2534,11 @@
       <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:8" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="33"/>
       <c r="H26" s="28"/>
     </row>
@@ -2546,27 +2546,27 @@
       <c r="H27" s="28"/>
     </row>
     <row r="28" spans="1:8" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="75" t="s">
+      <c r="A28" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="77" t="s">
+      <c r="B28" s="69"/>
+      <c r="C28" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="78"/>
-      <c r="E28" s="77" t="s">
+      <c r="D28" s="65"/>
+      <c r="E28" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="78"/>
+      <c r="F28" s="65"/>
       <c r="H28" s="28"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="79"/>
-      <c r="B29" s="79"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
       <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2624,8 +2624,8 @@
       <c r="H35" s="28"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="74"/>
-      <c r="B36" s="74"/>
+      <c r="A36" s="70"/>
+      <c r="B36" s="70"/>
       <c r="C36" s="61"/>
       <c r="D36" s="61"/>
       <c r="E36" s="61"/>
@@ -2633,8 +2633,8 @@
       <c r="H36" s="28"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="74"/>
-      <c r="B37" s="74"/>
+      <c r="A37" s="70"/>
+      <c r="B37" s="70"/>
       <c r="C37" s="61"/>
       <c r="D37" s="61"/>
       <c r="E37" s="61"/>
@@ -2642,8 +2642,8 @@
       <c r="H37" s="28"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="74"/>
-      <c r="B38" s="74"/>
+      <c r="A38" s="70"/>
+      <c r="B38" s="70"/>
       <c r="C38" s="61"/>
       <c r="D38" s="61"/>
       <c r="E38" s="61"/>
@@ -2720,6 +2720,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="A26:C26"/>
@@ -2736,55 +2785,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3761,36 +3761,34 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F43:G43"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A48:B48"/>
@@ -3807,34 +3805,36 @@
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C38:E38"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:G30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>